<commit_message>
nuevo dash, actualizacion en consulta, falta descarga de PDF
</commit_message>
<xml_diff>
--- a/tickets/tickets.xlsx
+++ b/tickets/tickets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -645,6 +645,34 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>lorenzo.orozco.garcia@gmail.com</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2024-08-27 16:23:26</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>pedro</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Problemon</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>No se como hacer geocerca</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>